<commit_message>
add visualizacao post mais recente
</commit_message>
<xml_diff>
--- a/dicionario_dados.xlsx
+++ b/dicionario_dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre Ejzenmesser\Desktop\Insper\6 Semestre\Megadados\bird_box\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A8481F-BB30-4CA7-8D77-CD2180228C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5EC48E-8B68-45BC-BC8C-2C5C57633DCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C3EC5F4-3C14-4469-9C3F-1E96F3910CCC}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Dicionario" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Dicionario!$A$1:$K$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Dicionario!$A$1:$K$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="80">
   <si>
     <t>usuario</t>
   </si>
@@ -255,21 +255,6 @@
     <t>CURRENT_TIMESTAMP</t>
   </si>
   <si>
-    <t>likes</t>
-  </si>
-  <si>
-    <t>deslikes</t>
-  </si>
-  <si>
-    <t>Quantidade total que o post teve de curtidas</t>
-  </si>
-  <si>
-    <t>Quantidade total que o post teve de não curtidas</t>
-  </si>
-  <si>
-    <t>DEFAULT 0</t>
-  </si>
-  <si>
     <t>liked</t>
   </si>
   <si>
@@ -283,6 +268,12 @@
   </si>
   <si>
     <t>Restrições</t>
+  </si>
+  <si>
+    <t>data_post</t>
+  </si>
+  <si>
+    <t>Data e hora em que o post foi feito pelo usuário</t>
   </si>
 </sst>
 </file>
@@ -437,7 +428,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -677,17 +668,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -695,19 +675,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -771,7 +738,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -891,52 +858,19 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -966,52 +900,76 @@
     <xf numFmtId="0" fontId="3" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1328,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879847A5-EB33-400D-A809-C074141973E9}">
-  <dimension ref="A1:K1048574"/>
+  <dimension ref="A1:K1048573"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="40" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1342,7 +1300,7 @@
     <col min="4" max="4" width="79.6640625" customWidth="1"/>
     <col min="5" max="5" width="30.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="7" max="7" width="41.6640625" customWidth="1"/>
     <col min="8" max="8" width="16.77734375" customWidth="1"/>
     <col min="9" max="9" width="22.77734375" customWidth="1"/>
     <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
@@ -1350,19 +1308,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="59"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="48"/>
     </row>
     <row r="2" spans="1:11" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -1396,14 +1354,14 @@
         <v>48</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="63" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -1435,8 +1393,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.3">
-      <c r="A4" s="42"/>
-      <c r="B4" s="45"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="64"/>
       <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
@@ -1466,8 +1424,8 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="43"/>
-      <c r="B5" s="46"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="12" t="s">
         <v>17</v>
       </c>
@@ -1531,11 +1489,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="42" x14ac:dyDescent="0.3">
-      <c r="A7" s="73" t="s">
+    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.3">
+      <c r="A7" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="55" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -1567,8 +1525,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.3">
-      <c r="A8" s="74"/>
-      <c r="B8" s="71"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="20" t="s">
         <v>19</v>
       </c>
@@ -1598,8 +1556,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.3">
-      <c r="A9" s="74"/>
-      <c r="B9" s="71"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="22" t="s">
         <v>20</v>
       </c>
@@ -1629,8 +1587,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.3">
-      <c r="A10" s="74"/>
-      <c r="B10" s="71"/>
+      <c r="A10" s="58"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="20" t="s">
         <v>21</v>
       </c>
@@ -1660,8 +1618,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.3">
-      <c r="A11" s="74"/>
-      <c r="B11" s="71"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="22" t="s">
         <v>22</v>
       </c>
@@ -1691,53 +1649,53 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.3">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="76" t="s">
+      <c r="A12" s="58"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="76" t="s">
+      <c r="D12" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="76" t="s">
+      <c r="E12" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="76" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="76" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="76" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="76" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="76" t="s">
+      <c r="F12" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="K12" s="77" t="s">
+      <c r="K12" s="44" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.3">
-      <c r="A13" s="74"/>
-      <c r="B13" s="71"/>
+    <row r="13" spans="1:11" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="58"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="22" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H13" s="22" t="s">
         <v>12</v>
@@ -1752,552 +1710,531 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="75"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="68" t="s">
+    <row r="14" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="67"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15" s="28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="73" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="71"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="72"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="50"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="51"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="76" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="58"/>
+      <c r="B23" s="77"/>
+      <c r="C23" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="58"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="58"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="58"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="58"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="42" x14ac:dyDescent="0.3">
+      <c r="A28" s="58"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="K28" s="42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="59"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="68" t="s">
+      <c r="E29" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="68" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="68" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="68" t="s">
-        <v>77</v>
-      </c>
-      <c r="H14" s="68" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="68" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="68" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="69" t="s">
+      <c r="H29" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="45" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="48"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="K16" s="28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="K17" s="30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="K18" s="32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="53"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="K19" s="34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="K20" s="36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="61"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K21" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="62"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="I22" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="J22" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" s="40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="73" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="78" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="K23" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="74"/>
-      <c r="B24" s="79"/>
-      <c r="C24" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="74"/>
-      <c r="B25" s="79"/>
-      <c r="C25" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I25" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="J25" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="K25" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="74"/>
-      <c r="B26" s="79"/>
-      <c r="C26" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J26" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="K26" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="74"/>
-      <c r="B27" s="79"/>
-      <c r="C27" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I27" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="J27" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="K27" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="74"/>
-      <c r="B28" s="79"/>
-      <c r="C28" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J28" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="K28" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="42" x14ac:dyDescent="0.3">
-      <c r="A29" s="74"/>
-      <c r="B29" s="79"/>
-      <c r="C29" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29" s="66" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="66" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="66" t="s">
-        <v>12</v>
-      </c>
-      <c r="I29" s="66" t="s">
-        <v>12</v>
-      </c>
-      <c r="J29" s="66" t="s">
-        <v>13</v>
-      </c>
-      <c r="K29" s="67" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="84.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="75"/>
-      <c r="B30" s="80"/>
-      <c r="C30" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F30" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="H30" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J30" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="K30" s="81" t="s">
-        <v>33</v>
-      </c>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="3"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -2307,7 +2244,6 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2352,38 +2288,29 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="1048574" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H1048574" s="1"/>
+    <row r="1048573" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H1048573" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="A22:A29"/>
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="A7:A13"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B23:B30"/>
-    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="42" fitToWidth="0" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="40" fitToWidth="0" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="30" max="19" man="1"/>
+    <brk id="29" max="19" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="11" max="29" man="1"/>

</xml_diff>